<commit_message>
NgocLV update cart future
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_codegym\Sprint-2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2BB484-FB69-4889-80C3-7CBF2A191856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A354EE2-AE45-4347-90AB-6C01899B287A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="3315" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{0C60A366-B985-451E-B931-40A0AE442565}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{0C60A366-B985-451E-B931-40A0AE442565}"/>
   </bookViews>
   <sheets>
     <sheet name="unit" sheetId="1" r:id="rId1"/>
     <sheet name="image" sheetId="2" r:id="rId2"/>
     <sheet name="category" sheetId="3" r:id="rId3"/>
     <sheet name="Food" sheetId="4" r:id="rId4"/>
+    <sheet name="roles" sheetId="5" r:id="rId5"/>
+    <sheet name="Customer" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -205,13 +207,259 @@
   </si>
   <si>
     <t>teen lop</t>
+  </si>
+  <si>
+    <t>id_roles</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>id_account</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>encrypt_password</t>
+  </si>
+  <si>
+    <t>flag_delete</t>
+  </si>
+  <si>
+    <t>username_account</t>
+  </si>
+  <si>
+    <t>van81@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$99tlxGF9KnBQuO.xhXLZDO1IAhsv/BsPzKfT04EyyDz9mTqXRj9.u</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Cẩm Vân</t>
+  </si>
+  <si>
+    <t>customer1</t>
+  </si>
+  <si>
+    <t>huy11@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$yF3uicEDL4b2WGa7ahS6J.0mUyQx15asKTRYJ81HsE98uoSlsmphS</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Huy</t>
+  </si>
+  <si>
+    <t>customer2</t>
+  </si>
+  <si>
+    <t>hocchh@gmai.com</t>
+  </si>
+  <si>
+    <t>$2a$10$oCaX.gKP4QVkicj9ahcQFuPh6ggMMr03awIFQspdS4vpTdCYtYdUG</t>
+  </si>
+  <si>
+    <t>Hồ Hải Học</t>
+  </si>
+  <si>
+    <t>customer3</t>
+  </si>
+  <si>
+    <t>haminh5@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$HGGHS04DdBvoQ3oRoPL48ukIvuSyu0uSbK/YF5mQ/dRdu9jlhSUlu</t>
+  </si>
+  <si>
+    <t>Trần Hà Minh</t>
+  </si>
+  <si>
+    <t>customer4</t>
+  </si>
+  <si>
+    <t>hiuminh@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$OfeDvClrmxkvgzLqYsU11OnKq2.gSoJMTApY1Q5psoCzFeJ66F7za</t>
+  </si>
+  <si>
+    <t>Hoàng Minh Hiếu</t>
+  </si>
+  <si>
+    <t>customer5</t>
+  </si>
+  <si>
+    <t>giangha@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$Cuasx7U4EtP4qkTqCcrBGuVB.Ng0P.R7rckFREQ0kmxDh/WzGyyMa</t>
+  </si>
+  <si>
+    <t>Hoàng Hà Giang</t>
+  </si>
+  <si>
+    <t>customer6</t>
+  </si>
+  <si>
+    <t>namthanh4@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$n5eKyesgvLxyJHhfpBjzve5Tbw.2v4.HVaI5/B/cyFQhLSq3tMkea</t>
+  </si>
+  <si>
+    <t>Hồ Nguyễn Nam Thành</t>
+  </si>
+  <si>
+    <t>customer7</t>
+  </si>
+  <si>
+    <t>phannhung@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$OTzHvGP3OwzTv.4vJKRrJOluJuLukHilFny5pnThGVcM9FpvHLcJe</t>
+  </si>
+  <si>
+    <t>Phan Thị Thùy Nhung</t>
+  </si>
+  <si>
+    <t>customer8</t>
+  </si>
+  <si>
+    <t>anhanh@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$92Sjci7it1nte3hiDkJUSOO9QhBdd9XRHz05vP1aVJlMiajDHMdmK</t>
+  </si>
+  <si>
+    <t>Lê Đức Anh</t>
+  </si>
+  <si>
+    <t>customer9</t>
+  </si>
+  <si>
+    <t>baohothai@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$KSxLbgXP7JYiKgx6pgkJl.KvJzE5bu2PPhPZkm2/zNtt.PVf1SfLy</t>
+  </si>
+  <si>
+    <t>Hồ Thái Bảo</t>
+  </si>
+  <si>
+    <t>customer10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>annguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$HhchRqEQdJVhmnz76e3y7efrCre48R58wHBYi1DYvgQZjvlzntine</t>
+  </si>
+  <si>
+    <t>account_role</t>
+  </si>
+  <si>
+    <t>account_id</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Lại Văn Ngọc</t>
+  </si>
+  <si>
+    <t>id_customer</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>account_id_account</t>
+  </si>
+  <si>
+    <t>12 Trần Hưng Đạo, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>87 Lê Lợi, Quảng Trị</t>
+  </si>
+  <si>
+    <t>100 Hùng Vương, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>08 Tiểu la, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>534 Lê Duẩn, Huế</t>
+  </si>
+  <si>
+    <t>788 Nguyễn Tất Thành, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>52 Nguyễn Huệ, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>02 Đống Đa, Quảng Nam</t>
+  </si>
+  <si>
+    <t>01 Phan Đình Phùng, Hà Nội</t>
+  </si>
+  <si>
+    <t>675 Nguyễn Chí Thanh, Quảng Trị</t>
+  </si>
+  <si>
+    <t>0912415515</t>
+  </si>
+  <si>
+    <t>0912112222</t>
+  </si>
+  <si>
+    <t>0975112911</t>
+  </si>
+  <si>
+    <t>0398666999</t>
+  </si>
+  <si>
+    <t>0905686868</t>
+  </si>
+  <si>
+    <t>0378987668</t>
+  </si>
+  <si>
+    <t>0901567987</t>
+  </si>
+  <si>
+    <t>0913812632</t>
+  </si>
+  <si>
+    <t>0975342423</t>
+  </si>
+  <si>
+    <t>0898922134</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +467,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +486,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,10 +538,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -273,15 +554,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,7 +891,7 @@
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63CB75C-B10C-4CD9-9303-AE905EACEC19}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +985,7 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -706,7 +1000,7 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
@@ -719,7 +1013,7 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -734,7 +1028,7 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
@@ -747,7 +1041,7 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -762,7 +1056,7 @@
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
@@ -775,7 +1069,7 @@
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -790,7 +1084,7 @@
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
@@ -803,7 +1097,7 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -818,7 +1112,7 @@
       <c r="E12">
         <v>5</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
@@ -831,7 +1125,7 @@
       <c r="E13">
         <v>6</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -846,7 +1140,7 @@
       <c r="E14">
         <v>6</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -859,7 +1153,7 @@
       <c r="E15">
         <v>7</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -874,7 +1168,7 @@
       <c r="E16">
         <v>7</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
@@ -887,7 +1181,7 @@
       <c r="E17">
         <v>8</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -902,7 +1196,7 @@
       <c r="E18">
         <v>8</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
@@ -915,7 +1209,7 @@
       <c r="E19">
         <v>9</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -930,7 +1224,7 @@
       <c r="E20">
         <v>9</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21">
@@ -942,7 +1236,7 @@
       <c r="E21">
         <v>10</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -956,7 +1250,7 @@
       <c r="E22">
         <v>10</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23">
@@ -968,7 +1262,7 @@
       <c r="E23">
         <v>11</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -982,7 +1276,7 @@
       <c r="E24">
         <v>11</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25">
@@ -994,7 +1288,7 @@
       <c r="E25">
         <v>12</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1008,7 +1302,7 @@
       <c r="E26">
         <v>12</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27">
@@ -1020,7 +1314,7 @@
       <c r="E27">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1034,7 +1328,7 @@
       <c r="E28">
         <v>13</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29">
@@ -1063,6 +1357,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
     <mergeCell ref="B3:B20"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="F23:F24"/>
@@ -1072,11 +1371,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1087,7 +1381,7 @@
   <dimension ref="C3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D10"/>
+      <selection activeCell="I21" sqref="H21:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1463,7 @@
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,4 +1484,649 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C380A3AD-FF28-4DBD-B0A2-D28370FC6A92}">
+  <dimension ref="C3:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="N3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="9">
+        <v>2</v>
+      </c>
+      <c r="P6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="9">
+        <v>3</v>
+      </c>
+      <c r="P7" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="9">
+        <v>4</v>
+      </c>
+      <c r="P8" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="9">
+        <v>5</v>
+      </c>
+      <c r="P9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="G10" s="9">
+        <v>6</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="9">
+        <v>6</v>
+      </c>
+      <c r="P10" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="G11" s="9">
+        <v>7</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="9">
+        <v>7</v>
+      </c>
+      <c r="P11" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+      <c r="G12" s="9">
+        <v>8</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="9">
+        <v>8</v>
+      </c>
+      <c r="P12" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13" s="9">
+        <v>9</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="9">
+        <v>9</v>
+      </c>
+      <c r="P13" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+      <c r="G14" s="9">
+        <v>10</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="9">
+        <v>10</v>
+      </c>
+      <c r="P14" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F15" s="5"/>
+      <c r="G15" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N15" s="5"/>
+      <c r="O15" s="9">
+        <v>11</v>
+      </c>
+      <c r="P15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{11CC7825-45CA-4851-9BA3-2F3F3F8E93EE}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{7F4D8266-3B66-4E24-98B3-C6BA988875D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD37161-67EC-4E48-8707-E2C26B19E8DB}">
+  <dimension ref="C4:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F16:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>7</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>8</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>9</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="9">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="9">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>